<commit_message>
comments , models changes , api , interface
</commit_message>
<xml_diff>
--- a/data v2 (O_o)/class.xlsx
+++ b/data v2 (O_o)/class.xlsx
@@ -1,40 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoomo\Desktop\last verssion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\new data set\Data labeled\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2AD37D70-0C4D-49DC-A754-D3054FE0AD4A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" xr2:uid="{528B2D74-1939-45A6-B510-C91E7DD6E594}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>curva_direita_agressiva</t>
   </si>
   <si>
+    <t>curva_esquerda_agressiva</t>
+  </si>
+  <si>
     <t>evento_nao_agressivo</t>
   </si>
   <si>
@@ -47,31 +45,19 @@
     <t>aceleracao_agressiva</t>
   </si>
   <si>
-    <t>aggressive right curve</t>
-  </si>
-  <si>
-    <t>curva_esquerda_agraaessiva</t>
-  </si>
-  <si>
-    <t>aggressive left turn</t>
-  </si>
-  <si>
-    <t>event_nao_aggressive</t>
-  </si>
-  <si>
-    <t>exchange aggressive right lane</t>
-  </si>
-  <si>
-    <t>aggressive braking</t>
-  </si>
-  <si>
-    <t>aggressive acceleration</t>
+    <t>event</t>
+  </si>
+  <si>
+    <t>val</t>
+  </si>
+  <si>
+    <t>troca_faixa_esquerda_agressiva</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -101,11 +87,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,88 +402,85 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56DC6DD-3CF7-4627-B236-B3754103FC00}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="38" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B8">
-    <sortCondition ref="B1"/>
+  <sortState ref="A2:B9">
+    <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>